<commit_message>
Reading the data from Excel sheet
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/bio.xlsx
+++ b/src/main/java/resources/excelsheet/bio.xlsx
@@ -55,7 +55,7 @@
     <t>Dinesh</t>
   </si>
   <si>
-    <t>22-03-1998</t>
+    <t>22-03-1994</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>